<commit_message>
Finished BookAppointment(error) and CaptureVitals
</commit_message>
<xml_diff>
--- a/Test scenario & Test case/TestCase_OpenMRS.xlsx
+++ b/Test scenario & Test case/TestCase_OpenMRS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\GitHub\OpenMRSTesting-SWT301\Test scenario &amp; Test case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B790DBB-4F81-426D-87DE-061251C914B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748B2B4C-ACED-4A7E-8139-ED7BE2ED0955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,11 @@
     <sheet name="View Patient" sheetId="5" r:id="rId5"/>
     <sheet name="Search Patient" sheetId="4" r:id="rId6"/>
     <sheet name="Book Appointment" sheetId="3" r:id="rId7"/>
+    <sheet name="Capture Vitals" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Book Appointment'!$A$1:$H$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Book Appointment'!$A$1:$H$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Capture Vitals'!$A$1:$H$32</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Find Patient Record'!$A$1:$H$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Login!$A$1:$H$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Logout!$A$1:$H$29</definedName>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="182">
   <si>
     <t>Test Steps</t>
   </si>
@@ -99,38 +101,664 @@
     <t>BA_004</t>
   </si>
   <si>
-    <t>BA_005</t>
-  </si>
-  <si>
     <t>Verify admin is able to book appointment for patient</t>
   </si>
   <si>
-    <t>Verify admin is unable to book appointment for patient when there is no appointment requests for patient</t>
+    <t>Verify admin is able to book appointment for patient when there is no appointment requests for patient</t>
   </si>
   <si>
-    <t>Verify admin is unable to book appointment for patient when there is no available time slots</t>
+    <t>Verify admin is unable to book appointment for patient when there is no available appointment of that type available</t>
+  </si>
+  <si>
+    <t>Verify admin can cancel a patient's appointment.</t>
   </si>
   <si>
     <t>Admin is logged into the system.
+Admin is on Manage Appointments Page.
 Patient has an appointment request.
-There is an appointment available in the time slots.</t>
+There is an appointment of the patient's type available.</t>
   </si>
   <si>
     <t>Admin is logged into the system.
+Admin is on Manage Appointments Page.
 Patient has no appointment requests.
 There is an appointment available in the time slots.</t>
   </si>
   <si>
     <t>Admin is logged into the system.
+Admin is on Manage Appointments Page.
 Patient has an appointment request.
-There is no appointment available in the time slots.</t>
+There is no appointment available of that type.</t>
+  </si>
+  <si>
+    <t>Admin is logged into the system.
+Admin is on Manage Appointments Page.
+Patient has an appointment scheduled in the schedule.</t>
+  </si>
+  <si>
+    <t>1. Input Patient ID into search menu
+2. Choose Patient
+3. Choose "Book this Appointment" next to the appointment that need to be booked
+4. Choose the appointment in the list of available appointments abd click "Next"
+5. Click "Save"</t>
+  </si>
+  <si>
+    <t>PatientID = "1001MH"
+Appointment type = "Gynecology"</t>
+  </si>
+  <si>
+    <t>1. Input Patient ID into search menu
+2. Choose Patient
+3. Input appointment type in "Select Service Type" and click "Search"
+4. Choose the appointment in the list of available appointments abd click "Next"
+5. Click "Save"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PatientID = "1001MH"
+</t>
+  </si>
+  <si>
+    <t>1. Input Patient ID into search menu
+2. Choose Patient
+3. Input appointment type in "Select Service Type" and click "Search"</t>
+  </si>
+  <si>
+    <t>PatientID = "1001MH"
+Appointment type = "Surgery"</t>
+  </si>
+  <si>
+    <t>CV_001</t>
+  </si>
+  <si>
+    <t>CV_002</t>
+  </si>
+  <si>
+    <t>CV_003</t>
+  </si>
+  <si>
+    <t>CV_004</t>
+  </si>
+  <si>
+    <t>CV_005</t>
+  </si>
+  <si>
+    <t>CV_006</t>
+  </si>
+  <si>
+    <t>CV_007</t>
+  </si>
+  <si>
+    <t>Verify Admin can capture vitals for a patient</t>
+  </si>
+  <si>
+    <t>Verify Height field cannot be below minimum</t>
+  </si>
+  <si>
+    <t>Verify Height field cannot be above maximum</t>
+  </si>
+  <si>
+    <t>Verify Height field must be number</t>
+  </si>
+  <si>
+    <t>CV_008</t>
+  </si>
+  <si>
+    <t>CV_009</t>
+  </si>
+  <si>
+    <t>CV_010</t>
+  </si>
+  <si>
+    <t>CV_011</t>
+  </si>
+  <si>
+    <t>CV_012</t>
+  </si>
+  <si>
+    <t>CV_013</t>
+  </si>
+  <si>
+    <t>CV_014</t>
+  </si>
+  <si>
+    <t>Verify Weight field cannot be below minimum</t>
+  </si>
+  <si>
+    <t>Verify Weight field cannot be above maximum</t>
+  </si>
+  <si>
+    <t>Verify Weight field must be number</t>
+  </si>
+  <si>
+    <t>Verify BMI is calculated when both Height and Weight is inputted</t>
+  </si>
+  <si>
+    <t>Verify BMI is not calculated when only Height is inputted</t>
+  </si>
+  <si>
+    <t>Verify BMI is not calculated when only Weight is inputted</t>
+  </si>
+  <si>
+    <t>Verify Tempetature field cannot be below minimum</t>
+  </si>
+  <si>
+    <t>Verify Tempetature field cannot be above maximum</t>
+  </si>
+  <si>
+    <t>Verify Tempetature field must be number</t>
+  </si>
+  <si>
+    <t>CV_015</t>
+  </si>
+  <si>
+    <t>CV_016</t>
+  </si>
+  <si>
+    <t>CV_017</t>
+  </si>
+  <si>
+    <t>CV_018</t>
+  </si>
+  <si>
+    <t>CV_019</t>
+  </si>
+  <si>
+    <t>Verify Pulse field cannot be below minimum</t>
+  </si>
+  <si>
+    <t>Verify Pulse field cannot be above maximum</t>
+  </si>
+  <si>
+    <t>Verify Pulse field must be number</t>
+  </si>
+  <si>
+    <t>CV_020</t>
+  </si>
+  <si>
+    <t>CV_021</t>
+  </si>
+  <si>
+    <t>CV_022</t>
+  </si>
+  <si>
+    <t>CV_023</t>
+  </si>
+  <si>
+    <t>CV_024</t>
+  </si>
+  <si>
+    <t>CV_025</t>
+  </si>
+  <si>
+    <t>CV_026</t>
+  </si>
+  <si>
+    <t>CV_027</t>
+  </si>
+  <si>
+    <t>CV_028</t>
+  </si>
+  <si>
+    <t>CV_029</t>
+  </si>
+  <si>
+    <t>CV_030</t>
+  </si>
+  <si>
+    <t>CV_031</t>
+  </si>
+  <si>
+    <t>Verify Respiratory rate field cannot be below minimum</t>
+  </si>
+  <si>
+    <t>Verify Respiratory rate field cannot be above maximum</t>
+  </si>
+  <si>
+    <t>Verify Respiratory rate field must be number</t>
+  </si>
+  <si>
+    <t>Verify Upper Blood Pressure field cannot be below minimum</t>
+  </si>
+  <si>
+    <t>Verify Upper Blood Pressure field cannot be above maximum</t>
+  </si>
+  <si>
+    <t>Verify Upper Blood Pressure field must be number</t>
+  </si>
+  <si>
+    <t>Verify Lower Blood Pressure field cannot be below minimum</t>
+  </si>
+  <si>
+    <t>Verify Lower Blood Pressure field cannot be above maximum</t>
+  </si>
+  <si>
+    <t>Verify Lower Blood Pressure field must be number</t>
+  </si>
+  <si>
+    <t>Verify Lower Blood Pressure field must be lower than Upper Blood Pressure</t>
+  </si>
+  <si>
+    <t>Verify Arterial blood oxygen saturation (pulse oximeter) field cannot be below minimum</t>
+  </si>
+  <si>
+    <t>Verify Arterial blood oxygen saturation (pulse oximeter) field cannot be above maximum</t>
+  </si>
+  <si>
+    <t>Verify Arterial blood oxygen saturation (pulse oximeter) field must be number</t>
+  </si>
+  <si>
+    <t>TestCase ID+G7A1:F7A1:H12B31A1:G6B31A1:G6A1:H17B31A1:G6A1:H21B31A1:G6A1:J21A1A1:I21</t>
+  </si>
+  <si>
+    <t>Verify Admin can cancel capture vitals for a patient</t>
+  </si>
+  <si>
+    <t>Admin is logged into the system.
+Admin is on the Capture Vitals Page.
+Patient is checked in.</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "No, Find Another Patient"</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Height, Weight, Temperature, Pulse, Respiratory rate, Upper and Lower Blood Pressure, Arterial blood oxygen saturation (pulse oximeter)
+5. Click "Save"
+5. On the Confirm page, click Save</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Height below minimum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Height above maximum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Height not a number value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Weight below minimum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Weight above maximum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Weight not a number value</t>
+  </si>
+  <si>
+    <t>Verify BMI is not calculated when neither Height and Weight is inputted</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Height and Weight
+5. Navigate to (Calculated) BMI tab</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Height 
+5. Navigate to (Calculated) BMI tab</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Weight
+5. Navigate to (Calculated) BMI tab</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4.Navigate to (Calculated) BMI tab</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Tempetature below minimum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Tempetature above maximum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Tempetature not a number value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Pulse below minimum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Pulse above maximum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Pulse not a number value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Respiratory rate below minimum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Respiratory rate above maximum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Respiratory rate not a number value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Upper Blood Pressure below minimum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Upper Blood Pressure above maximum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Upper Blood Pressure not a number value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Lower Blood Pressure below minimum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Lower Blood Pressure above maximum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Lower Blood Pressure not a number value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Upper Blood Pressure and Lower Blood Pressure</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Arterial blood oxygen saturation (pulse oximeter) below minimum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Arterial blood oxygen saturation (pulse oximeter) above maximum value</t>
+  </si>
+  <si>
+    <t>1. Input patient ID into search field
+2. Choose Patient
+3. Choose "Yes, Record Vitals"
+4. Input Arterial blood oxygen saturation (pulse oximeter) not a number value</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Height = 170
+Weight = 65
+Temperature = 37
+Pulse = 85
+Respratory rate = 20
+Upper Blood Pressure = 120
+Lower Blood Pressure = 80
+Arterial blood oxygen saturation (pulse oximeter) = 99</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Height = -1</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Height = a</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Height = 280</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Weight = -1</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Weight = 255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient ID = 1001MH
+Height = 170
+Weight = 65
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient ID = 1001MH
+Height = 170
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient ID = 1001MH
+Weight = 65
+</t>
+  </si>
+  <si>
+    <t>Patient's BMI is: 22.5</t>
+  </si>
+  <si>
+    <t>If you record a weight and height, we will calculate the BMI</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Temperature = 10</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Temperature = 50</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Temperature = a</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Pulse = -1</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Pulse = 250</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Pulse = a</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Respiratory rate = -1</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Respiratory rate = a</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Respiratory rate = 100</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Upper Blood Pressure = a</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Upper Blood Pressure = 300</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Upper Blood Pressure = -1</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Arterial blood oxygen saturation (pulse oximeter) = -2</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Arterial blood oxygen saturation (pulse oximeter) = a</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Arterial blood oxygen saturation (pulse oximeter) = 110</t>
+  </si>
+  <si>
+    <t>Entered Vitals for &lt;PatientName&gt;</t>
+  </si>
+  <si>
+    <t>Navigate back to Patient List</t>
+  </si>
+  <si>
+    <t>Minimum: 10</t>
+  </si>
+  <si>
+    <t>Maximum: 272</t>
+  </si>
+  <si>
+    <t>Must be a number</t>
+  </si>
+  <si>
+    <t>Minimum: 0</t>
+  </si>
+  <si>
+    <t>Maximum: 250</t>
+  </si>
+  <si>
+    <t>Minimum: 25</t>
+  </si>
+  <si>
+    <t>Maximum: 43</t>
+  </si>
+  <si>
+    <t>Must be a whole number</t>
+  </si>
+  <si>
+    <t>Maximum: 230</t>
+  </si>
+  <si>
+    <t>Maximum: 99</t>
+  </si>
+  <si>
+    <t>Minimum: 50</t>
+  </si>
+  <si>
+    <t>Maximum: 150</t>
+  </si>
+  <si>
+    <t>Maximum: 100</t>
+  </si>
+  <si>
+    <t>System allows us to continue</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>KietNHG</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Weight = a</t>
+  </si>
+  <si>
+    <t>Minimum: 30</t>
+  </si>
+  <si>
+    <t>Systolic blood pressure must be greater than Diastolic blood pressure</t>
+  </si>
+  <si>
+    <t>Scheduled an appointment for &lt;PatientName&gt;</t>
+  </si>
+  <si>
+    <t>Appointmtnt status updates from "Scheduled" to "Cancelled</t>
+  </si>
+  <si>
+    <t>1. Input Patient ID into search menu
+2. Choose Patient
+3. Choose "Cancel this Appointment" next to a scheduled appointment
+4. Click "</t>
+  </si>
+  <si>
+    <t>Patient ID = 1001MH
+Upper Blood Pressure = 80
+Lower Blood Pressure = 120</t>
+  </si>
+  <si>
+    <t>No available time slots</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -154,6 +782,11 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -188,7 +821,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -331,11 +964,152 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -392,6 +1166,39 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -15522,9 +16329,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V101"/>
+  <dimension ref="A1:V98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
@@ -15542,31 +16349,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="10" customFormat="1" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="22" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="9"/>
@@ -15583,22 +16390,34 @@
       <c r="U1" s="9"/>
       <c r="V1" s="9"/>
     </row>
-    <row r="2" spans="1:22" ht="53.25" customHeight="1">
+    <row r="2" spans="1:22" ht="90" thickBot="1">
       <c r="A2" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
+      <c r="D2" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>173</v>
+      </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -15613,22 +16432,34 @@
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
     </row>
-    <row r="3" spans="1:22" ht="53.25" customHeight="1">
+    <row r="3" spans="1:22" ht="89.25">
       <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="14"/>
+      <c r="D3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>173</v>
+      </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -15643,7 +16474,7 @@
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
     </row>
-    <row r="4" spans="1:22" ht="53.25" customHeight="1">
+    <row r="4" spans="1:22" ht="63.75">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -15651,14 +16482,26 @@
         <v>22</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="14"/>
+        <v>26</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>173</v>
+      </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -15673,18 +16516,34 @@
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
     </row>
-    <row r="5" spans="1:22" ht="53.25" customHeight="1">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:22" ht="53.25" customHeight="1" thickBot="1">
+      <c r="A5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="14"/>
+      <c r="B5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>173</v>
+      </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -15699,79 +16558,77 @@
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
     </row>
-    <row r="6" spans="1:22" ht="53.25" customHeight="1">
-      <c r="A6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-    </row>
-    <row r="7" spans="1:22" ht="53.25" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-    </row>
-    <row r="8" spans="1:22" ht="53.25" customHeight="1" thickBot="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
+    <row r="6" spans="1:22" ht="12.75" customHeight="1">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+    </row>
+    <row r="7" spans="1:22" ht="12.75" customHeight="1">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+    </row>
+    <row r="8" spans="1:22" ht="12.75" customHeight="1">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
     </row>
     <row r="9" spans="1:22" ht="12.75" customHeight="1">
       <c r="A9" s="4"/>
@@ -15829,7 +16686,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -15853,7 +16710,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="H12" s="6"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -15925,7 +16782,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -15973,7 +16830,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
@@ -15997,7 +16854,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -16117,7 +16974,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="6"/>
+      <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -16141,7 +16998,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="6"/>
+      <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -16165,7 +17022,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
+      <c r="H25" s="6"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -16181,7 +17038,7 @@
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
     </row>
-    <row r="26" spans="1:22" ht="12.75" customHeight="1">
+    <row r="26" spans="1:22">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -16189,7 +17046,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
+      <c r="H26" s="6"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -16205,7 +17062,7 @@
       <c r="U26" s="5"/>
       <c r="V26" s="5"/>
     </row>
-    <row r="27" spans="1:22" ht="12.75" customHeight="1">
+    <row r="27" spans="1:22">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -16229,7 +17086,7 @@
       <c r="U27" s="5"/>
       <c r="V27" s="5"/>
     </row>
-    <row r="28" spans="1:22" ht="12.75" customHeight="1">
+    <row r="28" spans="1:22">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -16237,7 +17094,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
-      <c r="H28" s="6"/>
+      <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -16261,7 +17118,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="6"/>
+      <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -16302,52 +17159,3012 @@
       <c r="V30" s="5"/>
     </row>
     <row r="31" spans="1:22">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
-      <c r="V31" s="5"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
     </row>
     <row r="32" spans="1:22">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
-      <c r="V32" s="5"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+    </row>
+    <row r="33" spans="1:22">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+    </row>
+    <row r="34" spans="1:22">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+    </row>
+    <row r="35" spans="1:22">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="3"/>
+    </row>
+    <row r="36" spans="1:22">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+    </row>
+    <row r="37" spans="1:22">
+      <c r="A37" s="2"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+    </row>
+    <row r="38" spans="1:22">
+      <c r="A38" s="2"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="3"/>
+    </row>
+    <row r="39" spans="1:22">
+      <c r="A39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+    </row>
+    <row r="40" spans="1:22">
+      <c r="A40" s="2"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
+      <c r="V40" s="3"/>
+    </row>
+    <row r="41" spans="1:22">
+      <c r="A41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="3"/>
+      <c r="U41" s="3"/>
+      <c r="V41" s="3"/>
+    </row>
+    <row r="42" spans="1:22">
+      <c r="A42" s="2"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3"/>
+    </row>
+    <row r="43" spans="1:22">
+      <c r="A43" s="2"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+    </row>
+    <row r="44" spans="1:22">
+      <c r="A44" s="2"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="3"/>
+      <c r="U44" s="3"/>
+      <c r="V44" s="3"/>
+    </row>
+    <row r="45" spans="1:22">
+      <c r="A45" s="2"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="3"/>
+      <c r="U45" s="3"/>
+      <c r="V45" s="3"/>
+    </row>
+    <row r="46" spans="1:22">
+      <c r="A46" s="2"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3"/>
+      <c r="T46" s="3"/>
+      <c r="U46" s="3"/>
+      <c r="V46" s="3"/>
+    </row>
+    <row r="47" spans="1:22">
+      <c r="A47" s="2"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3"/>
+      <c r="T47" s="3"/>
+      <c r="U47" s="3"/>
+      <c r="V47" s="3"/>
+    </row>
+    <row r="48" spans="1:22">
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="3"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="3"/>
+      <c r="T48" s="3"/>
+      <c r="U48" s="3"/>
+      <c r="V48" s="3"/>
+    </row>
+    <row r="49" spans="1:22">
+      <c r="A49" s="2"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="3"/>
+      <c r="U49" s="3"/>
+      <c r="V49" s="3"/>
+    </row>
+    <row r="50" spans="1:22">
+      <c r="A50" s="2"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="3"/>
+      <c r="U50" s="3"/>
+      <c r="V50" s="3"/>
+    </row>
+    <row r="51" spans="1:22">
+      <c r="A51" s="2"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
+      <c r="V51" s="3"/>
+    </row>
+    <row r="52" spans="1:22">
+      <c r="A52" s="2"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
+      <c r="U52" s="3"/>
+      <c r="V52" s="3"/>
+    </row>
+    <row r="53" spans="1:22">
+      <c r="A53" s="2"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
+      <c r="T53" s="3"/>
+      <c r="U53" s="3"/>
+      <c r="V53" s="3"/>
+    </row>
+    <row r="54" spans="1:22">
+      <c r="A54" s="2"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="3"/>
+      <c r="R54" s="3"/>
+      <c r="S54" s="3"/>
+      <c r="T54" s="3"/>
+      <c r="U54" s="3"/>
+      <c r="V54" s="3"/>
+    </row>
+    <row r="55" spans="1:22">
+      <c r="A55" s="2"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="O55" s="3"/>
+      <c r="P55" s="3"/>
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="3"/>
+      <c r="T55" s="3"/>
+      <c r="U55" s="3"/>
+      <c r="V55" s="3"/>
+    </row>
+    <row r="56" spans="1:22">
+      <c r="A56" s="2"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3"/>
+      <c r="T56" s="3"/>
+      <c r="U56" s="3"/>
+      <c r="V56" s="3"/>
+    </row>
+    <row r="57" spans="1:22">
+      <c r="A57" s="2"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="3"/>
+      <c r="T57" s="3"/>
+      <c r="U57" s="3"/>
+      <c r="V57" s="3"/>
+    </row>
+    <row r="58" spans="1:22">
+      <c r="A58" s="2"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="3"/>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
+    </row>
+    <row r="59" spans="1:22">
+      <c r="A59" s="2"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="3"/>
+      <c r="T59" s="3"/>
+      <c r="U59" s="3"/>
+      <c r="V59" s="3"/>
+    </row>
+    <row r="60" spans="1:22">
+      <c r="A60" s="2"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="3"/>
+      <c r="T60" s="3"/>
+      <c r="U60" s="3"/>
+      <c r="V60" s="3"/>
+    </row>
+    <row r="61" spans="1:22">
+      <c r="A61" s="2"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="3"/>
+      <c r="O61" s="3"/>
+      <c r="P61" s="3"/>
+      <c r="Q61" s="3"/>
+      <c r="R61" s="3"/>
+      <c r="S61" s="3"/>
+      <c r="T61" s="3"/>
+      <c r="U61" s="3"/>
+      <c r="V61" s="3"/>
+    </row>
+    <row r="62" spans="1:22">
+      <c r="A62" s="2"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="3"/>
+      <c r="T62" s="3"/>
+      <c r="U62" s="3"/>
+      <c r="V62" s="3"/>
+    </row>
+    <row r="63" spans="1:22">
+      <c r="A63" s="2"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="3"/>
+      <c r="T63" s="3"/>
+      <c r="U63" s="3"/>
+      <c r="V63" s="3"/>
+    </row>
+    <row r="64" spans="1:22">
+      <c r="A64" s="2"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
+      <c r="M64" s="3"/>
+      <c r="N64" s="3"/>
+      <c r="O64" s="3"/>
+      <c r="P64" s="3"/>
+      <c r="Q64" s="3"/>
+      <c r="R64" s="3"/>
+      <c r="S64" s="3"/>
+      <c r="T64" s="3"/>
+      <c r="U64" s="3"/>
+      <c r="V64" s="3"/>
+    </row>
+    <row r="65" spans="1:22">
+      <c r="A65" s="2"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+      <c r="P65" s="3"/>
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="3"/>
+      <c r="T65" s="3"/>
+      <c r="U65" s="3"/>
+      <c r="V65" s="3"/>
+    </row>
+    <row r="66" spans="1:22">
+      <c r="A66" s="2"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+      <c r="P66" s="3"/>
+      <c r="Q66" s="3"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="3"/>
+      <c r="T66" s="3"/>
+      <c r="U66" s="3"/>
+      <c r="V66" s="3"/>
+    </row>
+    <row r="67" spans="1:22">
+      <c r="A67" s="2"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="3"/>
+      <c r="T67" s="3"/>
+      <c r="U67" s="3"/>
+      <c r="V67" s="3"/>
+    </row>
+    <row r="68" spans="1:22">
+      <c r="A68" s="2"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="3"/>
+      <c r="T68" s="3"/>
+      <c r="U68" s="3"/>
+      <c r="V68" s="3"/>
+    </row>
+    <row r="69" spans="1:22">
+      <c r="A69" s="2"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="3"/>
+      <c r="N69" s="3"/>
+      <c r="O69" s="3"/>
+      <c r="P69" s="3"/>
+      <c r="Q69" s="3"/>
+      <c r="R69" s="3"/>
+      <c r="S69" s="3"/>
+      <c r="T69" s="3"/>
+      <c r="U69" s="3"/>
+      <c r="V69" s="3"/>
+    </row>
+    <row r="70" spans="1:22">
+      <c r="A70" s="2"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="3"/>
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="3"/>
+      <c r="T70" s="3"/>
+      <c r="U70" s="3"/>
+      <c r="V70" s="3"/>
+    </row>
+    <row r="71" spans="1:22">
+      <c r="A71" s="2"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="3"/>
+      <c r="O71" s="3"/>
+      <c r="P71" s="3"/>
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="3"/>
+      <c r="T71" s="3"/>
+      <c r="U71" s="3"/>
+      <c r="V71" s="3"/>
+    </row>
+    <row r="72" spans="1:22">
+      <c r="A72" s="2"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
+      <c r="M72" s="3"/>
+      <c r="N72" s="3"/>
+      <c r="O72" s="3"/>
+      <c r="P72" s="3"/>
+      <c r="Q72" s="3"/>
+      <c r="R72" s="3"/>
+      <c r="S72" s="3"/>
+      <c r="T72" s="3"/>
+      <c r="U72" s="3"/>
+      <c r="V72" s="3"/>
+    </row>
+    <row r="73" spans="1:22">
+      <c r="A73" s="2"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3"/>
+      <c r="N73" s="3"/>
+      <c r="O73" s="3"/>
+      <c r="P73" s="3"/>
+      <c r="Q73" s="3"/>
+      <c r="R73" s="3"/>
+      <c r="S73" s="3"/>
+      <c r="T73" s="3"/>
+      <c r="U73" s="3"/>
+      <c r="V73" s="3"/>
+    </row>
+    <row r="74" spans="1:22">
+      <c r="A74" s="2"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+      <c r="M74" s="3"/>
+      <c r="N74" s="3"/>
+      <c r="O74" s="3"/>
+      <c r="P74" s="3"/>
+      <c r="Q74" s="3"/>
+      <c r="R74" s="3"/>
+      <c r="S74" s="3"/>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+      <c r="V74" s="3"/>
+    </row>
+    <row r="75" spans="1:22">
+      <c r="A75" s="2"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="3"/>
+      <c r="P75" s="3"/>
+      <c r="Q75" s="3"/>
+      <c r="R75" s="3"/>
+      <c r="S75" s="3"/>
+      <c r="T75" s="3"/>
+      <c r="U75" s="3"/>
+      <c r="V75" s="3"/>
+    </row>
+    <row r="76" spans="1:22">
+      <c r="A76" s="2"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3"/>
+      <c r="N76" s="3"/>
+      <c r="O76" s="3"/>
+      <c r="P76" s="3"/>
+      <c r="Q76" s="3"/>
+      <c r="R76" s="3"/>
+      <c r="S76" s="3"/>
+      <c r="T76" s="3"/>
+      <c r="U76" s="3"/>
+      <c r="V76" s="3"/>
+    </row>
+    <row r="77" spans="1:22">
+      <c r="A77" s="2"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+      <c r="N77" s="3"/>
+      <c r="O77" s="3"/>
+      <c r="P77" s="3"/>
+      <c r="Q77" s="3"/>
+      <c r="R77" s="3"/>
+      <c r="S77" s="3"/>
+      <c r="T77" s="3"/>
+      <c r="U77" s="3"/>
+      <c r="V77" s="3"/>
+    </row>
+    <row r="78" spans="1:22">
+      <c r="A78" s="2"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="3"/>
+      <c r="P78" s="3"/>
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="3"/>
+      <c r="T78" s="3"/>
+      <c r="U78" s="3"/>
+      <c r="V78" s="3"/>
+    </row>
+    <row r="79" spans="1:22">
+      <c r="A79" s="2"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+      <c r="M79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="O79" s="3"/>
+      <c r="P79" s="3"/>
+      <c r="Q79" s="3"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="3"/>
+      <c r="T79" s="3"/>
+      <c r="U79" s="3"/>
+      <c r="V79" s="3"/>
+    </row>
+    <row r="80" spans="1:22">
+      <c r="A80" s="2"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="M80" s="3"/>
+      <c r="N80" s="3"/>
+      <c r="O80" s="3"/>
+      <c r="P80" s="3"/>
+      <c r="Q80" s="3"/>
+      <c r="R80" s="3"/>
+      <c r="S80" s="3"/>
+      <c r="T80" s="3"/>
+      <c r="U80" s="3"/>
+      <c r="V80" s="3"/>
+    </row>
+    <row r="81" spans="1:22">
+      <c r="A81" s="2"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
+      <c r="K81" s="3"/>
+      <c r="L81" s="3"/>
+      <c r="M81" s="3"/>
+      <c r="N81" s="3"/>
+      <c r="O81" s="3"/>
+      <c r="P81" s="3"/>
+      <c r="Q81" s="3"/>
+      <c r="R81" s="3"/>
+      <c r="S81" s="3"/>
+      <c r="T81" s="3"/>
+      <c r="U81" s="3"/>
+      <c r="V81" s="3"/>
+    </row>
+    <row r="82" spans="1:22">
+      <c r="A82" s="2"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
+      <c r="M82" s="3"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="3"/>
+      <c r="P82" s="3"/>
+      <c r="Q82" s="3"/>
+      <c r="R82" s="3"/>
+      <c r="S82" s="3"/>
+      <c r="T82" s="3"/>
+      <c r="U82" s="3"/>
+      <c r="V82" s="3"/>
+    </row>
+    <row r="83" spans="1:22">
+      <c r="A83" s="2"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
+      <c r="M83" s="3"/>
+      <c r="N83" s="3"/>
+      <c r="O83" s="3"/>
+      <c r="P83" s="3"/>
+      <c r="Q83" s="3"/>
+      <c r="R83" s="3"/>
+      <c r="S83" s="3"/>
+      <c r="T83" s="3"/>
+      <c r="U83" s="3"/>
+      <c r="V83" s="3"/>
+    </row>
+    <row r="84" spans="1:22">
+      <c r="A84" s="2"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="3"/>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+      <c r="L84" s="3"/>
+      <c r="M84" s="3"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="3"/>
+      <c r="P84" s="3"/>
+      <c r="Q84" s="3"/>
+      <c r="R84" s="3"/>
+      <c r="S84" s="3"/>
+      <c r="T84" s="3"/>
+      <c r="U84" s="3"/>
+      <c r="V84" s="3"/>
+    </row>
+    <row r="85" spans="1:22">
+      <c r="A85" s="2"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="3"/>
+      <c r="L85" s="3"/>
+      <c r="M85" s="3"/>
+      <c r="N85" s="3"/>
+      <c r="O85" s="3"/>
+      <c r="P85" s="3"/>
+      <c r="Q85" s="3"/>
+      <c r="R85" s="3"/>
+      <c r="S85" s="3"/>
+      <c r="T85" s="3"/>
+      <c r="U85" s="3"/>
+      <c r="V85" s="3"/>
+    </row>
+    <row r="86" spans="1:22">
+      <c r="A86" s="2"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="3"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="3"/>
+      <c r="P86" s="3"/>
+      <c r="Q86" s="3"/>
+      <c r="R86" s="3"/>
+      <c r="S86" s="3"/>
+      <c r="T86" s="3"/>
+      <c r="U86" s="3"/>
+      <c r="V86" s="3"/>
+    </row>
+    <row r="87" spans="1:22">
+      <c r="A87" s="2"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="I87" s="3"/>
+      <c r="J87" s="3"/>
+      <c r="K87" s="3"/>
+      <c r="L87" s="3"/>
+      <c r="M87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="O87" s="3"/>
+      <c r="P87" s="3"/>
+      <c r="Q87" s="3"/>
+      <c r="R87" s="3"/>
+      <c r="S87" s="3"/>
+      <c r="T87" s="3"/>
+      <c r="U87" s="3"/>
+      <c r="V87" s="3"/>
+    </row>
+    <row r="88" spans="1:22">
+      <c r="A88" s="2"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="3"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="3"/>
+      <c r="P88" s="3"/>
+      <c r="Q88" s="3"/>
+      <c r="R88" s="3"/>
+      <c r="S88" s="3"/>
+      <c r="T88" s="3"/>
+      <c r="U88" s="3"/>
+      <c r="V88" s="3"/>
+    </row>
+    <row r="89" spans="1:22">
+      <c r="A89" s="2"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+      <c r="K89" s="3"/>
+      <c r="L89" s="3"/>
+      <c r="M89" s="3"/>
+      <c r="N89" s="3"/>
+      <c r="O89" s="3"/>
+      <c r="P89" s="3"/>
+      <c r="Q89" s="3"/>
+      <c r="R89" s="3"/>
+      <c r="S89" s="3"/>
+      <c r="T89" s="3"/>
+      <c r="U89" s="3"/>
+      <c r="V89" s="3"/>
+    </row>
+    <row r="90" spans="1:22">
+      <c r="A90" s="2"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="3"/>
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+      <c r="P90" s="3"/>
+      <c r="Q90" s="3"/>
+      <c r="R90" s="3"/>
+      <c r="S90" s="3"/>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
+    </row>
+    <row r="91" spans="1:22">
+      <c r="A91" s="2"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
+      <c r="P91" s="3"/>
+      <c r="Q91" s="3"/>
+      <c r="R91" s="3"/>
+      <c r="S91" s="3"/>
+      <c r="T91" s="3"/>
+      <c r="U91" s="3"/>
+      <c r="V91" s="3"/>
+    </row>
+    <row r="92" spans="1:22">
+      <c r="A92" s="2"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+      <c r="M92" s="3"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="3"/>
+      <c r="P92" s="3"/>
+      <c r="Q92" s="3"/>
+      <c r="R92" s="3"/>
+      <c r="S92" s="3"/>
+      <c r="T92" s="3"/>
+      <c r="U92" s="3"/>
+      <c r="V92" s="3"/>
+    </row>
+    <row r="93" spans="1:22">
+      <c r="A93" s="2"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
+      <c r="I93" s="3"/>
+      <c r="J93" s="3"/>
+      <c r="K93" s="3"/>
+      <c r="L93" s="3"/>
+      <c r="M93" s="3"/>
+      <c r="N93" s="3"/>
+      <c r="O93" s="3"/>
+      <c r="P93" s="3"/>
+      <c r="Q93" s="3"/>
+      <c r="R93" s="3"/>
+      <c r="S93" s="3"/>
+      <c r="T93" s="3"/>
+      <c r="U93" s="3"/>
+      <c r="V93" s="3"/>
+    </row>
+    <row r="94" spans="1:22">
+      <c r="A94" s="2"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
+      <c r="I94" s="3"/>
+      <c r="J94" s="3"/>
+      <c r="K94" s="3"/>
+      <c r="L94" s="3"/>
+      <c r="M94" s="3"/>
+      <c r="N94" s="3"/>
+      <c r="O94" s="3"/>
+      <c r="P94" s="3"/>
+      <c r="Q94" s="3"/>
+      <c r="R94" s="3"/>
+      <c r="S94" s="3"/>
+      <c r="T94" s="3"/>
+      <c r="U94" s="3"/>
+      <c r="V94" s="3"/>
+    </row>
+    <row r="95" spans="1:22">
+      <c r="A95" s="2"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
+      <c r="I95" s="3"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="3"/>
+      <c r="L95" s="3"/>
+      <c r="M95" s="3"/>
+      <c r="N95" s="3"/>
+      <c r="O95" s="3"/>
+      <c r="P95" s="3"/>
+      <c r="Q95" s="3"/>
+      <c r="R95" s="3"/>
+      <c r="S95" s="3"/>
+      <c r="T95" s="3"/>
+      <c r="U95" s="3"/>
+      <c r="V95" s="3"/>
+    </row>
+    <row r="96" spans="1:22">
+      <c r="A96" s="2"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
+      <c r="I96" s="3"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="3"/>
+      <c r="M96" s="3"/>
+      <c r="N96" s="3"/>
+      <c r="O96" s="3"/>
+      <c r="P96" s="3"/>
+      <c r="Q96" s="3"/>
+      <c r="R96" s="3"/>
+      <c r="S96" s="3"/>
+      <c r="T96" s="3"/>
+      <c r="U96" s="3"/>
+      <c r="V96" s="3"/>
+    </row>
+    <row r="97" spans="1:22">
+      <c r="A97" s="2"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
+      <c r="I97" s="3"/>
+      <c r="J97" s="3"/>
+      <c r="K97" s="3"/>
+      <c r="L97" s="3"/>
+      <c r="M97" s="3"/>
+      <c r="N97" s="3"/>
+      <c r="O97" s="3"/>
+      <c r="P97" s="3"/>
+      <c r="Q97" s="3"/>
+      <c r="R97" s="3"/>
+      <c r="S97" s="3"/>
+      <c r="T97" s="3"/>
+      <c r="U97" s="3"/>
+      <c r="V97" s="3"/>
+    </row>
+    <row r="98" spans="1:22">
+      <c r="A98" s="2"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="3"/>
+      <c r="I98" s="3"/>
+      <c r="J98" s="3"/>
+      <c r="K98" s="3"/>
+      <c r="L98" s="3"/>
+      <c r="M98" s="3"/>
+      <c r="N98" s="3"/>
+      <c r="O98" s="3"/>
+      <c r="P98" s="3"/>
+      <c r="Q98" s="3"/>
+      <c r="R98" s="3"/>
+      <c r="S98" s="3"/>
+      <c r="T98" s="3"/>
+      <c r="U98" s="3"/>
+      <c r="V98" s="3"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H26" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4370754C-20B4-466D-A61C-6270F937E29C}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:V101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="38" style="1" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" style="1" customWidth="1"/>
+    <col min="8" max="22" width="17.28515625" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="14.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="10" customFormat="1" ht="12.75" customHeight="1" thickBot="1">
+      <c r="A1" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+    </row>
+    <row r="2" spans="1:22" ht="127.5">
+      <c r="A2" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+    </row>
+    <row r="3" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A3" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+    </row>
+    <row r="4" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A4" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+    </row>
+    <row r="5" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A5" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+    </row>
+    <row r="6" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A6" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+    </row>
+    <row r="7" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A7" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+    </row>
+    <row r="8" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A8" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+    </row>
+    <row r="9" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A9" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+    </row>
+    <row r="10" spans="1:22" ht="63.75">
+      <c r="A10" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+    </row>
+    <row r="11" spans="1:22" ht="63.75">
+      <c r="A11" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+    </row>
+    <row r="12" spans="1:22" ht="63.75">
+      <c r="A12" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+    </row>
+    <row r="13" spans="1:22" ht="51">
+      <c r="A13" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+    </row>
+    <row r="14" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A14" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+    </row>
+    <row r="15" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A15" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+    </row>
+    <row r="16" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A16" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+    </row>
+    <row r="17" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A17" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+    </row>
+    <row r="18" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A18" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+    </row>
+    <row r="19" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A19" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+    </row>
+    <row r="20" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A20" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I20" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+    </row>
+    <row r="21" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A21" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I21" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+    </row>
+    <row r="22" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A22" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I22" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+    </row>
+    <row r="23" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A23" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I23" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+    </row>
+    <row r="24" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A24" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+    </row>
+    <row r="25" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A25" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I25" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+    </row>
+    <row r="26" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A26" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I26" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+    </row>
+    <row r="27" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A27" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I27" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+    </row>
+    <row r="28" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A28" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I28" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+    </row>
+    <row r="29" spans="1:22" ht="63.75">
+      <c r="A29" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="I29" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+    </row>
+    <row r="30" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A30" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="H30" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I30" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+    </row>
+    <row r="31" spans="1:22" ht="53.25" customHeight="1">
+      <c r="A31" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+    </row>
+    <row r="32" spans="1:22" ht="63.75">
+      <c r="A32" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="H32" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I32" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
     </row>
     <row r="33" spans="1:22">
       <c r="A33" s="4"/>
@@ -18006,8 +21823,9 @@
       <c r="V101" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H29" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <autoFilter ref="A1:H32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>